<commit_message>
Se agregaron mas datos en la plantilla
</commit_message>
<xml_diff>
--- a/extras/docs/Plantilla para Revision de Software.xlsx
+++ b/extras/docs/Plantilla para Revision de Software.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Error</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Url (Direccion en la que se encontro el problema)</t>
+  </si>
+  <si>
+    <t>Fecha de revision</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -130,11 +133,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -145,6 +174,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:H200"/>
+  <dimension ref="D3:I200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +498,7 @@
     <col min="7" max="7" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
@@ -476,8 +514,11 @@
       <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D4" s="2">
         <v>1</v>
       </c>
@@ -485,8 +526,9 @@
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <f>D4+1</f>
         <v>2</v>
@@ -495,18 +537,20 @@
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
-        <f t="shared" ref="D6:D9" si="0">D5+1</f>
+        <f t="shared" ref="D6:D69" si="0">D5+1</f>
         <v>3</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -515,8 +559,9 @@
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -525,8 +570,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -535,1343 +581,2108 @@
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
       <c r="G10" s="3"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="2"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
       <c r="G13" s="3"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="2"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
       <c r="G15" s="3"/>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="2"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="2"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="2"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
       <c r="G19" s="3"/>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="2"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="2"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
       <c r="G21" s="3"/>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D22" s="2"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="2"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
       <c r="G23" s="3"/>
       <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="2"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
       <c r="G24" s="3"/>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="2"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="2"/>
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="2"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="2"/>
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="2"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="2"/>
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="2"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
       <c r="E28" s="3"/>
       <c r="F28" s="2"/>
       <c r="G28" s="3"/>
       <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="2"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
       <c r="E29" s="3"/>
       <c r="F29" s="2"/>
       <c r="G29" s="3"/>
       <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="2"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="2"/>
       <c r="G30" s="3"/>
       <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D31" s="2"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" s="2"/>
       <c r="G31" s="3"/>
       <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="2"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="2"/>
       <c r="G32" s="3"/>
       <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D33" s="2"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="E33" s="3"/>
       <c r="F33" s="2"/>
       <c r="G33" s="3"/>
       <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="2"/>
       <c r="G34" s="3"/>
       <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="2"/>
       <c r="G35" s="3"/>
       <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="2"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="2"/>
       <c r="G36" s="3"/>
       <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="2"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="2"/>
       <c r="G37" s="3"/>
       <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D38" s="2"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="2"/>
       <c r="G38" s="3"/>
       <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="2"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="E39" s="3"/>
       <c r="F39" s="2"/>
       <c r="G39" s="3"/>
       <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="2"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
       <c r="E40" s="3"/>
       <c r="F40" s="2"/>
       <c r="G40" s="3"/>
       <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D41" s="2"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="2"/>
       <c r="G41" s="3"/>
       <c r="H41" s="2"/>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="2"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
       <c r="E42" s="3"/>
       <c r="F42" s="2"/>
       <c r="G42" s="3"/>
       <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D43" s="2"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
       <c r="E43" s="3"/>
       <c r="F43" s="2"/>
       <c r="G43" s="3"/>
       <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D44" s="2"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
       <c r="E44" s="3"/>
       <c r="F44" s="2"/>
       <c r="G44" s="3"/>
       <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D45" s="2"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
       <c r="E45" s="3"/>
       <c r="F45" s="2"/>
       <c r="G45" s="3"/>
       <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="2"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
       <c r="E46" s="3"/>
       <c r="F46" s="2"/>
       <c r="G46" s="3"/>
       <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="2"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
       <c r="E47" s="3"/>
       <c r="F47" s="2"/>
       <c r="G47" s="3"/>
       <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D48" s="2"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
       <c r="E48" s="3"/>
       <c r="F48" s="2"/>
       <c r="G48" s="3"/>
       <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D49" s="2"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
       <c r="E49" s="3"/>
       <c r="F49" s="2"/>
       <c r="G49" s="3"/>
       <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D50" s="2"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
       <c r="E50" s="3"/>
       <c r="F50" s="2"/>
       <c r="G50" s="3"/>
       <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D51" s="2"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
       <c r="E51" s="3"/>
       <c r="F51" s="2"/>
       <c r="G51" s="3"/>
       <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D52" s="2"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="2"/>
       <c r="G52" s="3"/>
       <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D53" s="2"/>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
       <c r="E53" s="3"/>
       <c r="F53" s="2"/>
       <c r="G53" s="3"/>
       <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D54" s="2"/>
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
       <c r="E54" s="3"/>
       <c r="F54" s="2"/>
       <c r="G54" s="3"/>
       <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D55" s="2"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D55" s="2">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
       <c r="E55" s="3"/>
       <c r="F55" s="2"/>
       <c r="G55" s="3"/>
       <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D56" s="2"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D56" s="2">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
       <c r="E56" s="3"/>
       <c r="F56" s="2"/>
       <c r="G56" s="3"/>
       <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D57" s="2"/>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D57" s="2">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
       <c r="E57" s="3"/>
       <c r="F57" s="2"/>
       <c r="G57" s="3"/>
       <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D58" s="2"/>
+      <c r="I57" s="6"/>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D58" s="2">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
       <c r="E58" s="3"/>
       <c r="F58" s="2"/>
       <c r="G58" s="3"/>
       <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D59" s="2"/>
+      <c r="I58" s="6"/>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D59" s="2">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
       <c r="E59" s="3"/>
       <c r="F59" s="2"/>
       <c r="G59" s="3"/>
       <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D60" s="2"/>
+      <c r="I59" s="6"/>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D60" s="2">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
       <c r="E60" s="3"/>
       <c r="F60" s="2"/>
       <c r="G60" s="3"/>
       <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D61" s="2"/>
+      <c r="I60" s="6"/>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D61" s="2">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
       <c r="E61" s="3"/>
       <c r="F61" s="2"/>
       <c r="G61" s="3"/>
       <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D62" s="2"/>
+      <c r="I61" s="6"/>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D62" s="2">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
       <c r="E62" s="3"/>
       <c r="F62" s="2"/>
       <c r="G62" s="3"/>
       <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D63" s="2"/>
+      <c r="I62" s="6"/>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D63" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
       <c r="E63" s="3"/>
       <c r="F63" s="2"/>
       <c r="G63" s="3"/>
       <c r="H63" s="2"/>
-    </row>
-    <row r="64" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D64" s="2"/>
+      <c r="I63" s="6"/>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D64" s="2">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
       <c r="E64" s="3"/>
       <c r="F64" s="2"/>
       <c r="G64" s="3"/>
       <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D65" s="2"/>
+      <c r="I64" s="6"/>
+    </row>
+    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D65" s="2">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
       <c r="E65" s="3"/>
       <c r="F65" s="2"/>
       <c r="G65" s="3"/>
       <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D66" s="2"/>
+      <c r="I65" s="6"/>
+    </row>
+    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D66" s="2">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
       <c r="E66" s="3"/>
       <c r="F66" s="2"/>
       <c r="G66" s="3"/>
       <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D67" s="2"/>
+      <c r="I66" s="6"/>
+    </row>
+    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D67" s="2">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
       <c r="E67" s="3"/>
       <c r="F67" s="2"/>
       <c r="G67" s="3"/>
       <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D68" s="2"/>
+      <c r="I67" s="6"/>
+    </row>
+    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D68" s="2">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
       <c r="E68" s="3"/>
       <c r="F68" s="2"/>
       <c r="G68" s="3"/>
       <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D69" s="2"/>
+      <c r="I68" s="6"/>
+    </row>
+    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D69" s="2">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
       <c r="E69" s="3"/>
       <c r="F69" s="2"/>
       <c r="G69" s="3"/>
       <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D70" s="2"/>
+      <c r="I69" s="6"/>
+    </row>
+    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D70" s="2">
+        <f>D69+1</f>
+        <v>67</v>
+      </c>
       <c r="E70" s="3"/>
       <c r="F70" s="2"/>
       <c r="G70" s="3"/>
       <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D71" s="2"/>
+      <c r="I70" s="6"/>
+    </row>
+    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D71" s="2">
+        <f t="shared" ref="D71:D134" si="1">D70+1</f>
+        <v>68</v>
+      </c>
       <c r="E71" s="3"/>
       <c r="F71" s="2"/>
       <c r="G71" s="3"/>
       <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="2"/>
+      <c r="I71" s="6"/>
+    </row>
+    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D72" s="2">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
       <c r="E72" s="3"/>
       <c r="F72" s="2"/>
       <c r="G72" s="3"/>
       <c r="H72" s="2"/>
-    </row>
-    <row r="73" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="2"/>
+      <c r="I72" s="6"/>
+    </row>
+    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D73" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
       <c r="E73" s="3"/>
       <c r="F73" s="2"/>
       <c r="G73" s="3"/>
       <c r="H73" s="2"/>
-    </row>
-    <row r="74" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D74" s="2"/>
+      <c r="I73" s="6"/>
+    </row>
+    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D74" s="2">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
       <c r="E74" s="3"/>
       <c r="F74" s="2"/>
       <c r="G74" s="3"/>
       <c r="H74" s="2"/>
-    </row>
-    <row r="75" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D75" s="2"/>
+      <c r="I74" s="6"/>
+    </row>
+    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D75" s="2">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
       <c r="E75" s="3"/>
       <c r="F75" s="2"/>
       <c r="G75" s="3"/>
       <c r="H75" s="2"/>
-    </row>
-    <row r="76" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D76" s="2"/>
+      <c r="I75" s="6"/>
+    </row>
+    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D76" s="2">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
       <c r="E76" s="3"/>
       <c r="F76" s="2"/>
       <c r="G76" s="3"/>
       <c r="H76" s="2"/>
-    </row>
-    <row r="77" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D77" s="2"/>
+      <c r="I76" s="6"/>
+    </row>
+    <row r="77" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D77" s="2">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
       <c r="E77" s="3"/>
       <c r="F77" s="2"/>
       <c r="G77" s="3"/>
       <c r="H77" s="2"/>
-    </row>
-    <row r="78" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D78" s="2"/>
+      <c r="I77" s="6"/>
+    </row>
+    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D78" s="2">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
       <c r="E78" s="3"/>
       <c r="F78" s="2"/>
       <c r="G78" s="3"/>
       <c r="H78" s="2"/>
-    </row>
-    <row r="79" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D79" s="2"/>
+      <c r="I78" s="6"/>
+    </row>
+    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D79" s="2">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
       <c r="E79" s="3"/>
       <c r="F79" s="2"/>
       <c r="G79" s="3"/>
       <c r="H79" s="2"/>
-    </row>
-    <row r="80" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D80" s="2"/>
+      <c r="I79" s="6"/>
+    </row>
+    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D80" s="2">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
       <c r="E80" s="3"/>
       <c r="F80" s="2"/>
       <c r="G80" s="3"/>
       <c r="H80" s="2"/>
-    </row>
-    <row r="81" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D81" s="2"/>
+      <c r="I80" s="6"/>
+    </row>
+    <row r="81" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D81" s="2">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
       <c r="E81" s="3"/>
       <c r="F81" s="2"/>
       <c r="G81" s="3"/>
       <c r="H81" s="2"/>
-    </row>
-    <row r="82" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D82" s="2"/>
+      <c r="I81" s="6"/>
+    </row>
+    <row r="82" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D82" s="2">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
       <c r="E82" s="3"/>
       <c r="F82" s="2"/>
       <c r="G82" s="3"/>
       <c r="H82" s="2"/>
-    </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D83" s="2"/>
+      <c r="I82" s="6"/>
+    </row>
+    <row r="83" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D83" s="2">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
       <c r="E83" s="3"/>
       <c r="F83" s="2"/>
       <c r="G83" s="3"/>
       <c r="H83" s="2"/>
-    </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D84" s="2"/>
+      <c r="I83" s="6"/>
+    </row>
+    <row r="84" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D84" s="2">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
       <c r="E84" s="3"/>
       <c r="F84" s="2"/>
       <c r="G84" s="3"/>
       <c r="H84" s="2"/>
-    </row>
-    <row r="85" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D85" s="2"/>
+      <c r="I84" s="6"/>
+    </row>
+    <row r="85" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D85" s="2">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
       <c r="E85" s="3"/>
       <c r="F85" s="2"/>
       <c r="G85" s="3"/>
       <c r="H85" s="2"/>
-    </row>
-    <row r="86" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D86" s="2"/>
+      <c r="I85" s="6"/>
+    </row>
+    <row r="86" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D86" s="2">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
       <c r="E86" s="3"/>
       <c r="F86" s="2"/>
       <c r="G86" s="3"/>
       <c r="H86" s="2"/>
-    </row>
-    <row r="87" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D87" s="2"/>
+      <c r="I86" s="6"/>
+    </row>
+    <row r="87" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D87" s="2">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
       <c r="E87" s="3"/>
       <c r="F87" s="2"/>
       <c r="G87" s="3"/>
       <c r="H87" s="2"/>
-    </row>
-    <row r="88" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D88" s="2"/>
+      <c r="I87" s="6"/>
+    </row>
+    <row r="88" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D88" s="2">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
       <c r="E88" s="3"/>
       <c r="F88" s="2"/>
       <c r="G88" s="3"/>
       <c r="H88" s="2"/>
-    </row>
-    <row r="89" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D89" s="2"/>
+      <c r="I88" s="6"/>
+    </row>
+    <row r="89" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D89" s="2">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
       <c r="E89" s="3"/>
       <c r="F89" s="2"/>
       <c r="G89" s="3"/>
       <c r="H89" s="2"/>
-    </row>
-    <row r="90" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D90" s="2"/>
+      <c r="I89" s="6"/>
+    </row>
+    <row r="90" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D90" s="2">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="2"/>
       <c r="G90" s="3"/>
       <c r="H90" s="2"/>
-    </row>
-    <row r="91" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D91" s="2"/>
+      <c r="I90" s="6"/>
+    </row>
+    <row r="91" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D91" s="2">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="2"/>
       <c r="G91" s="3"/>
       <c r="H91" s="2"/>
-    </row>
-    <row r="92" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D92" s="2"/>
+      <c r="I91" s="6"/>
+    </row>
+    <row r="92" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D92" s="2">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="2"/>
       <c r="G92" s="3"/>
       <c r="H92" s="2"/>
-    </row>
-    <row r="93" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D93" s="2"/>
+      <c r="I92" s="6"/>
+    </row>
+    <row r="93" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D93" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
       <c r="E93" s="3"/>
       <c r="F93" s="2"/>
       <c r="G93" s="3"/>
       <c r="H93" s="2"/>
-    </row>
-    <row r="94" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D94" s="2"/>
+      <c r="I93" s="6"/>
+    </row>
+    <row r="94" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D94" s="2">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
       <c r="E94" s="3"/>
       <c r="F94" s="2"/>
       <c r="G94" s="3"/>
       <c r="H94" s="2"/>
-    </row>
-    <row r="95" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D95" s="2"/>
+      <c r="I94" s="6"/>
+    </row>
+    <row r="95" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D95" s="2">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
       <c r="E95" s="3"/>
       <c r="F95" s="2"/>
       <c r="G95" s="3"/>
       <c r="H95" s="2"/>
-    </row>
-    <row r="96" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D96" s="2"/>
+      <c r="I95" s="6"/>
+    </row>
+    <row r="96" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D96" s="2">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
       <c r="E96" s="3"/>
       <c r="F96" s="2"/>
       <c r="G96" s="3"/>
       <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D97" s="2"/>
+      <c r="I96" s="6"/>
+    </row>
+    <row r="97" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D97" s="2">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
       <c r="E97" s="3"/>
       <c r="F97" s="2"/>
       <c r="G97" s="3"/>
       <c r="H97" s="2"/>
-    </row>
-    <row r="98" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D98" s="2"/>
+      <c r="I97" s="6"/>
+    </row>
+    <row r="98" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D98" s="2">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
       <c r="E98" s="3"/>
       <c r="F98" s="2"/>
       <c r="G98" s="3"/>
       <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D99" s="2"/>
+      <c r="I98" s="6"/>
+    </row>
+    <row r="99" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D99" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
       <c r="E99" s="3"/>
       <c r="F99" s="2"/>
       <c r="G99" s="3"/>
       <c r="H99" s="2"/>
-    </row>
-    <row r="100" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D100" s="2"/>
+      <c r="I99" s="6"/>
+    </row>
+    <row r="100" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D100" s="2">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
       <c r="E100" s="3"/>
       <c r="F100" s="2"/>
       <c r="G100" s="3"/>
       <c r="H100" s="2"/>
-    </row>
-    <row r="101" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D101" s="2"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="101" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D101" s="2">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
       <c r="E101" s="3"/>
       <c r="F101" s="2"/>
       <c r="G101" s="3"/>
       <c r="H101" s="2"/>
-    </row>
-    <row r="102" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D102" s="2"/>
+      <c r="I101" s="6"/>
+    </row>
+    <row r="102" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D102" s="2">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
       <c r="E102" s="3"/>
       <c r="F102" s="2"/>
       <c r="G102" s="3"/>
       <c r="H102" s="2"/>
-    </row>
-    <row r="103" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D103" s="2"/>
+      <c r="I102" s="6"/>
+    </row>
+    <row r="103" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D103" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
       <c r="E103" s="3"/>
       <c r="F103" s="2"/>
       <c r="G103" s="3"/>
       <c r="H103" s="2"/>
-    </row>
-    <row r="104" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D104" s="2"/>
+      <c r="I103" s="6"/>
+    </row>
+    <row r="104" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D104" s="2">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
       <c r="E104" s="3"/>
       <c r="F104" s="2"/>
       <c r="G104" s="3"/>
       <c r="H104" s="2"/>
-    </row>
-    <row r="105" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D105" s="2"/>
+      <c r="I104" s="6"/>
+    </row>
+    <row r="105" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D105" s="2">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
       <c r="E105" s="3"/>
       <c r="F105" s="2"/>
       <c r="G105" s="3"/>
       <c r="H105" s="2"/>
-    </row>
-    <row r="106" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D106" s="2"/>
+      <c r="I105" s="6"/>
+    </row>
+    <row r="106" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D106" s="2">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
       <c r="E106" s="3"/>
       <c r="F106" s="2"/>
       <c r="G106" s="3"/>
       <c r="H106" s="2"/>
-    </row>
-    <row r="107" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D107" s="2"/>
+      <c r="I106" s="6"/>
+    </row>
+    <row r="107" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D107" s="2">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
       <c r="E107" s="3"/>
       <c r="F107" s="2"/>
       <c r="G107" s="3"/>
       <c r="H107" s="2"/>
-    </row>
-    <row r="108" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D108" s="2"/>
+      <c r="I107" s="6"/>
+    </row>
+    <row r="108" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D108" s="2">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
       <c r="E108" s="3"/>
       <c r="F108" s="2"/>
       <c r="G108" s="3"/>
       <c r="H108" s="2"/>
-    </row>
-    <row r="109" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D109" s="2"/>
+      <c r="I108" s="6"/>
+    </row>
+    <row r="109" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D109" s="2">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
       <c r="E109" s="3"/>
       <c r="F109" s="2"/>
       <c r="G109" s="3"/>
       <c r="H109" s="2"/>
-    </row>
-    <row r="110" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D110" s="2"/>
+      <c r="I109" s="6"/>
+    </row>
+    <row r="110" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D110" s="2">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
       <c r="E110" s="3"/>
       <c r="F110" s="2"/>
       <c r="G110" s="3"/>
       <c r="H110" s="2"/>
-    </row>
-    <row r="111" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D111" s="2"/>
+      <c r="I110" s="6"/>
+    </row>
+    <row r="111" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D111" s="2">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
       <c r="E111" s="3"/>
       <c r="F111" s="2"/>
       <c r="G111" s="3"/>
       <c r="H111" s="2"/>
-    </row>
-    <row r="112" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D112" s="2"/>
+      <c r="I111" s="6"/>
+    </row>
+    <row r="112" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D112" s="2">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
       <c r="E112" s="3"/>
       <c r="F112" s="2"/>
       <c r="G112" s="3"/>
       <c r="H112" s="2"/>
-    </row>
-    <row r="113" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D113" s="2"/>
+      <c r="I112" s="6"/>
+    </row>
+    <row r="113" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D113" s="2">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
       <c r="E113" s="3"/>
       <c r="F113" s="2"/>
       <c r="G113" s="3"/>
       <c r="H113" s="2"/>
-    </row>
-    <row r="114" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D114" s="2"/>
+      <c r="I113" s="6"/>
+    </row>
+    <row r="114" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D114" s="2">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
       <c r="E114" s="3"/>
       <c r="F114" s="2"/>
       <c r="G114" s="3"/>
       <c r="H114" s="2"/>
-    </row>
-    <row r="115" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D115" s="2"/>
+      <c r="I114" s="6"/>
+    </row>
+    <row r="115" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D115" s="2">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
       <c r="E115" s="3"/>
       <c r="F115" s="2"/>
       <c r="G115" s="3"/>
       <c r="H115" s="2"/>
-    </row>
-    <row r="116" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D116" s="2"/>
+      <c r="I115" s="6"/>
+    </row>
+    <row r="116" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D116" s="2">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
       <c r="E116" s="3"/>
       <c r="F116" s="2"/>
       <c r="G116" s="3"/>
       <c r="H116" s="2"/>
-    </row>
-    <row r="117" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D117" s="2"/>
+      <c r="I116" s="6"/>
+    </row>
+    <row r="117" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D117" s="2">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
       <c r="E117" s="3"/>
       <c r="F117" s="2"/>
       <c r="G117" s="3"/>
       <c r="H117" s="2"/>
-    </row>
-    <row r="118" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D118" s="2"/>
+      <c r="I117" s="6"/>
+    </row>
+    <row r="118" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D118" s="2">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
       <c r="E118" s="3"/>
       <c r="F118" s="2"/>
       <c r="G118" s="3"/>
       <c r="H118" s="2"/>
-    </row>
-    <row r="119" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D119" s="2"/>
+      <c r="I118" s="6"/>
+    </row>
+    <row r="119" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D119" s="2">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
       <c r="E119" s="3"/>
       <c r="F119" s="2"/>
       <c r="G119" s="3"/>
       <c r="H119" s="2"/>
-    </row>
-    <row r="120" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D120" s="2"/>
+      <c r="I119" s="6"/>
+    </row>
+    <row r="120" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D120" s="2">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
       <c r="E120" s="3"/>
       <c r="F120" s="2"/>
       <c r="G120" s="3"/>
       <c r="H120" s="2"/>
-    </row>
-    <row r="121" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D121" s="2"/>
+      <c r="I120" s="6"/>
+    </row>
+    <row r="121" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D121" s="2">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
       <c r="E121" s="3"/>
       <c r="F121" s="2"/>
       <c r="G121" s="3"/>
       <c r="H121" s="2"/>
-    </row>
-    <row r="122" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D122" s="2"/>
+      <c r="I121" s="6"/>
+    </row>
+    <row r="122" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D122" s="2">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
       <c r="E122" s="3"/>
       <c r="F122" s="2"/>
       <c r="G122" s="3"/>
       <c r="H122" s="2"/>
-    </row>
-    <row r="123" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D123" s="2"/>
+      <c r="I122" s="6"/>
+    </row>
+    <row r="123" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D123" s="2">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
       <c r="E123" s="3"/>
       <c r="F123" s="2"/>
       <c r="G123" s="3"/>
       <c r="H123" s="2"/>
-    </row>
-    <row r="124" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D124" s="2"/>
+      <c r="I123" s="6"/>
+    </row>
+    <row r="124" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D124" s="2">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
       <c r="E124" s="3"/>
       <c r="F124" s="2"/>
       <c r="G124" s="3"/>
       <c r="H124" s="2"/>
-    </row>
-    <row r="125" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D125" s="2"/>
+      <c r="I124" s="6"/>
+    </row>
+    <row r="125" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D125" s="2">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
       <c r="E125" s="3"/>
       <c r="F125" s="2"/>
       <c r="G125" s="3"/>
       <c r="H125" s="2"/>
-    </row>
-    <row r="126" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D126" s="2"/>
+      <c r="I125" s="6"/>
+    </row>
+    <row r="126" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D126" s="2">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
       <c r="E126" s="3"/>
       <c r="F126" s="2"/>
       <c r="G126" s="3"/>
       <c r="H126" s="2"/>
-    </row>
-    <row r="127" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D127" s="2"/>
+      <c r="I126" s="6"/>
+    </row>
+    <row r="127" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D127" s="2">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
       <c r="E127" s="3"/>
       <c r="F127" s="2"/>
       <c r="G127" s="3"/>
       <c r="H127" s="2"/>
-    </row>
-    <row r="128" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D128" s="2"/>
+      <c r="I127" s="6"/>
+    </row>
+    <row r="128" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D128" s="2">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
       <c r="E128" s="3"/>
       <c r="F128" s="2"/>
       <c r="G128" s="3"/>
       <c r="H128" s="2"/>
-    </row>
-    <row r="129" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D129" s="2"/>
+      <c r="I128" s="6"/>
+    </row>
+    <row r="129" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D129" s="2">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
       <c r="E129" s="3"/>
       <c r="F129" s="2"/>
       <c r="G129" s="3"/>
       <c r="H129" s="2"/>
-    </row>
-    <row r="130" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D130" s="2"/>
+      <c r="I129" s="6"/>
+    </row>
+    <row r="130" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D130" s="2">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
       <c r="E130" s="3"/>
       <c r="F130" s="2"/>
       <c r="G130" s="3"/>
       <c r="H130" s="2"/>
-    </row>
-    <row r="131" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D131" s="2"/>
+      <c r="I130" s="6"/>
+    </row>
+    <row r="131" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D131" s="2">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
       <c r="E131" s="3"/>
       <c r="F131" s="2"/>
       <c r="G131" s="3"/>
       <c r="H131" s="2"/>
-    </row>
-    <row r="132" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D132" s="2"/>
+      <c r="I131" s="6"/>
+    </row>
+    <row r="132" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D132" s="2">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
       <c r="E132" s="3"/>
       <c r="F132" s="2"/>
       <c r="G132" s="3"/>
       <c r="H132" s="2"/>
-    </row>
-    <row r="133" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D133" s="2"/>
+      <c r="I132" s="6"/>
+    </row>
+    <row r="133" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D133" s="2">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
       <c r="E133" s="3"/>
       <c r="F133" s="2"/>
       <c r="G133" s="3"/>
       <c r="H133" s="2"/>
-    </row>
-    <row r="134" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D134" s="2"/>
+      <c r="I133" s="6"/>
+    </row>
+    <row r="134" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D134" s="2">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
       <c r="E134" s="3"/>
       <c r="F134" s="2"/>
       <c r="G134" s="3"/>
       <c r="H134" s="2"/>
-    </row>
-    <row r="135" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D135" s="2"/>
+      <c r="I134" s="6"/>
+    </row>
+    <row r="135" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D135" s="2">
+        <f t="shared" ref="D135:D198" si="2">D134+1</f>
+        <v>132</v>
+      </c>
       <c r="E135" s="3"/>
       <c r="F135" s="2"/>
       <c r="G135" s="3"/>
       <c r="H135" s="2"/>
-    </row>
-    <row r="136" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D136" s="2"/>
+      <c r="I135" s="6"/>
+    </row>
+    <row r="136" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D136" s="2">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
       <c r="E136" s="3"/>
       <c r="F136" s="2"/>
       <c r="G136" s="3"/>
       <c r="H136" s="2"/>
-    </row>
-    <row r="137" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D137" s="2"/>
+      <c r="I136" s="6"/>
+    </row>
+    <row r="137" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D137" s="2">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
       <c r="E137" s="3"/>
       <c r="F137" s="2"/>
       <c r="G137" s="3"/>
       <c r="H137" s="2"/>
-    </row>
-    <row r="138" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D138" s="2"/>
+      <c r="I137" s="6"/>
+    </row>
+    <row r="138" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D138" s="2">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
       <c r="E138" s="3"/>
       <c r="F138" s="2"/>
       <c r="G138" s="3"/>
       <c r="H138" s="2"/>
-    </row>
-    <row r="139" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D139" s="2"/>
+      <c r="I138" s="6"/>
+    </row>
+    <row r="139" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D139" s="2">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
       <c r="E139" s="3"/>
       <c r="F139" s="2"/>
       <c r="G139" s="3"/>
       <c r="H139" s="2"/>
-    </row>
-    <row r="140" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D140" s="2"/>
+      <c r="I139" s="6"/>
+    </row>
+    <row r="140" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D140" s="2">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
       <c r="E140" s="3"/>
       <c r="F140" s="2"/>
       <c r="G140" s="3"/>
       <c r="H140" s="2"/>
-    </row>
-    <row r="141" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D141" s="2"/>
+      <c r="I140" s="6"/>
+    </row>
+    <row r="141" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D141" s="2">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
       <c r="E141" s="3"/>
       <c r="F141" s="2"/>
       <c r="G141" s="3"/>
       <c r="H141" s="2"/>
-    </row>
-    <row r="142" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D142" s="2"/>
+      <c r="I141" s="6"/>
+    </row>
+    <row r="142" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D142" s="2">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
       <c r="E142" s="3"/>
       <c r="F142" s="2"/>
       <c r="G142" s="3"/>
       <c r="H142" s="2"/>
-    </row>
-    <row r="143" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D143" s="2"/>
+      <c r="I142" s="6"/>
+    </row>
+    <row r="143" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D143" s="2">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
       <c r="E143" s="3"/>
       <c r="F143" s="2"/>
       <c r="G143" s="3"/>
       <c r="H143" s="2"/>
-    </row>
-    <row r="144" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D144" s="2"/>
+      <c r="I143" s="6"/>
+    </row>
+    <row r="144" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D144" s="2">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
       <c r="E144" s="3"/>
       <c r="F144" s="2"/>
       <c r="G144" s="3"/>
       <c r="H144" s="2"/>
-    </row>
-    <row r="145" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D145" s="2"/>
+      <c r="I144" s="6"/>
+    </row>
+    <row r="145" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D145" s="2">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
       <c r="E145" s="3"/>
       <c r="F145" s="2"/>
       <c r="G145" s="3"/>
       <c r="H145" s="2"/>
-    </row>
-    <row r="146" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D146" s="2"/>
+      <c r="I145" s="6"/>
+    </row>
+    <row r="146" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D146" s="2">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
       <c r="E146" s="3"/>
       <c r="F146" s="2"/>
       <c r="G146" s="3"/>
       <c r="H146" s="2"/>
-    </row>
-    <row r="147" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D147" s="2"/>
+      <c r="I146" s="6"/>
+    </row>
+    <row r="147" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D147" s="2">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
       <c r="E147" s="3"/>
       <c r="F147" s="2"/>
       <c r="G147" s="3"/>
       <c r="H147" s="2"/>
-    </row>
-    <row r="148" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D148" s="2"/>
+      <c r="I147" s="6"/>
+    </row>
+    <row r="148" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D148" s="2">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
       <c r="E148" s="3"/>
       <c r="F148" s="2"/>
       <c r="G148" s="3"/>
       <c r="H148" s="2"/>
-    </row>
-    <row r="149" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D149" s="2"/>
+      <c r="I148" s="6"/>
+    </row>
+    <row r="149" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D149" s="2">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
       <c r="E149" s="3"/>
       <c r="F149" s="2"/>
       <c r="G149" s="3"/>
       <c r="H149" s="2"/>
-    </row>
-    <row r="150" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D150" s="2"/>
+      <c r="I149" s="6"/>
+    </row>
+    <row r="150" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D150" s="2">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
       <c r="E150" s="3"/>
       <c r="F150" s="2"/>
       <c r="G150" s="3"/>
       <c r="H150" s="2"/>
-    </row>
-    <row r="151" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D151" s="2"/>
+      <c r="I150" s="6"/>
+    </row>
+    <row r="151" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D151" s="2">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
       <c r="E151" s="3"/>
       <c r="F151" s="2"/>
       <c r="G151" s="3"/>
       <c r="H151" s="2"/>
-    </row>
-    <row r="152" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D152" s="2"/>
+      <c r="I151" s="6"/>
+    </row>
+    <row r="152" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D152" s="2">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
       <c r="E152" s="3"/>
       <c r="F152" s="2"/>
       <c r="G152" s="3"/>
       <c r="H152" s="2"/>
-    </row>
-    <row r="153" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D153" s="2"/>
+      <c r="I152" s="6"/>
+    </row>
+    <row r="153" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D153" s="2">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
       <c r="E153" s="3"/>
       <c r="F153" s="2"/>
       <c r="G153" s="3"/>
       <c r="H153" s="2"/>
-    </row>
-    <row r="154" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D154" s="2"/>
+      <c r="I153" s="6"/>
+    </row>
+    <row r="154" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D154" s="2">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
       <c r="E154" s="3"/>
       <c r="F154" s="2"/>
       <c r="G154" s="3"/>
       <c r="H154" s="2"/>
-    </row>
-    <row r="155" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D155" s="2"/>
+      <c r="I154" s="6"/>
+    </row>
+    <row r="155" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D155" s="2">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
       <c r="E155" s="3"/>
       <c r="F155" s="2"/>
       <c r="G155" s="3"/>
       <c r="H155" s="2"/>
-    </row>
-    <row r="156" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D156" s="2"/>
+      <c r="I155" s="6"/>
+    </row>
+    <row r="156" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D156" s="2">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
       <c r="E156" s="3"/>
       <c r="F156" s="2"/>
       <c r="G156" s="3"/>
       <c r="H156" s="2"/>
-    </row>
-    <row r="157" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D157" s="2"/>
+      <c r="I156" s="6"/>
+    </row>
+    <row r="157" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D157" s="2">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
       <c r="E157" s="3"/>
       <c r="F157" s="2"/>
       <c r="G157" s="3"/>
       <c r="H157" s="2"/>
-    </row>
-    <row r="158" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D158" s="2"/>
+      <c r="I157" s="6"/>
+    </row>
+    <row r="158" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D158" s="2">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
       <c r="E158" s="3"/>
       <c r="F158" s="2"/>
       <c r="G158" s="3"/>
       <c r="H158" s="2"/>
-    </row>
-    <row r="159" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D159" s="2"/>
+      <c r="I158" s="6"/>
+    </row>
+    <row r="159" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D159" s="2">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
       <c r="E159" s="3"/>
       <c r="F159" s="2"/>
       <c r="G159" s="3"/>
       <c r="H159" s="2"/>
-    </row>
-    <row r="160" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D160" s="2"/>
+      <c r="I159" s="6"/>
+    </row>
+    <row r="160" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D160" s="2">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
       <c r="E160" s="3"/>
       <c r="F160" s="2"/>
       <c r="G160" s="3"/>
       <c r="H160" s="2"/>
-    </row>
-    <row r="161" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D161" s="2"/>
+      <c r="I160" s="6"/>
+    </row>
+    <row r="161" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D161" s="2">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
       <c r="E161" s="3"/>
       <c r="F161" s="2"/>
       <c r="G161" s="3"/>
       <c r="H161" s="2"/>
-    </row>
-    <row r="162" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D162" s="2"/>
+      <c r="I161" s="6"/>
+    </row>
+    <row r="162" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D162" s="2">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
       <c r="E162" s="3"/>
       <c r="F162" s="2"/>
       <c r="G162" s="3"/>
       <c r="H162" s="2"/>
-    </row>
-    <row r="163" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D163" s="2"/>
+      <c r="I162" s="6"/>
+    </row>
+    <row r="163" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D163" s="2">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
       <c r="E163" s="3"/>
       <c r="F163" s="2"/>
       <c r="G163" s="3"/>
       <c r="H163" s="2"/>
-    </row>
-    <row r="164" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D164" s="2"/>
+      <c r="I163" s="6"/>
+    </row>
+    <row r="164" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D164" s="2">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
       <c r="E164" s="3"/>
       <c r="F164" s="2"/>
       <c r="G164" s="3"/>
       <c r="H164" s="2"/>
-    </row>
-    <row r="165" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D165" s="2"/>
+      <c r="I164" s="6"/>
+    </row>
+    <row r="165" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D165" s="2">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
       <c r="E165" s="3"/>
       <c r="F165" s="2"/>
       <c r="G165" s="3"/>
       <c r="H165" s="2"/>
-    </row>
-    <row r="166" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D166" s="2"/>
+      <c r="I165" s="6"/>
+    </row>
+    <row r="166" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D166" s="2">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
       <c r="E166" s="3"/>
       <c r="F166" s="2"/>
       <c r="G166" s="3"/>
       <c r="H166" s="2"/>
-    </row>
-    <row r="167" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D167" s="2"/>
+      <c r="I166" s="6"/>
+    </row>
+    <row r="167" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D167" s="2">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
       <c r="E167" s="3"/>
       <c r="F167" s="2"/>
       <c r="G167" s="3"/>
       <c r="H167" s="2"/>
-    </row>
-    <row r="168" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D168" s="2"/>
+      <c r="I167" s="6"/>
+    </row>
+    <row r="168" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D168" s="2">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
       <c r="E168" s="3"/>
       <c r="F168" s="2"/>
       <c r="G168" s="3"/>
       <c r="H168" s="2"/>
-    </row>
-    <row r="169" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D169" s="2"/>
+      <c r="I168" s="6"/>
+    </row>
+    <row r="169" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D169" s="2">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
       <c r="E169" s="3"/>
       <c r="F169" s="2"/>
       <c r="G169" s="3"/>
       <c r="H169" s="2"/>
-    </row>
-    <row r="170" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D170" s="2"/>
+      <c r="I169" s="6"/>
+    </row>
+    <row r="170" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D170" s="2">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
       <c r="E170" s="3"/>
       <c r="F170" s="2"/>
       <c r="G170" s="3"/>
       <c r="H170" s="2"/>
-    </row>
-    <row r="171" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D171" s="2"/>
+      <c r="I170" s="6"/>
+    </row>
+    <row r="171" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D171" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
       <c r="E171" s="3"/>
       <c r="F171" s="2"/>
       <c r="G171" s="3"/>
       <c r="H171" s="2"/>
-    </row>
-    <row r="172" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D172" s="2"/>
+      <c r="I171" s="6"/>
+    </row>
+    <row r="172" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D172" s="2">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
       <c r="E172" s="3"/>
       <c r="F172" s="2"/>
       <c r="G172" s="3"/>
       <c r="H172" s="2"/>
-    </row>
-    <row r="173" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D173" s="2"/>
+      <c r="I172" s="6"/>
+    </row>
+    <row r="173" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D173" s="2">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
       <c r="E173" s="3"/>
       <c r="F173" s="2"/>
       <c r="G173" s="3"/>
       <c r="H173" s="2"/>
-    </row>
-    <row r="174" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D174" s="2"/>
+      <c r="I173" s="6"/>
+    </row>
+    <row r="174" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D174" s="2">
+        <f t="shared" si="2"/>
+        <v>171</v>
+      </c>
       <c r="E174" s="3"/>
       <c r="F174" s="2"/>
       <c r="G174" s="3"/>
       <c r="H174" s="2"/>
-    </row>
-    <row r="175" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D175" s="2"/>
+      <c r="I174" s="6"/>
+    </row>
+    <row r="175" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D175" s="2">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
       <c r="E175" s="3"/>
       <c r="F175" s="2"/>
       <c r="G175" s="3"/>
       <c r="H175" s="2"/>
-    </row>
-    <row r="176" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D176" s="2"/>
+      <c r="I175" s="6"/>
+    </row>
+    <row r="176" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D176" s="2">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
       <c r="E176" s="3"/>
       <c r="F176" s="2"/>
       <c r="G176" s="3"/>
       <c r="H176" s="2"/>
-    </row>
-    <row r="177" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D177" s="2"/>
+      <c r="I176" s="6"/>
+    </row>
+    <row r="177" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D177" s="2">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
       <c r="E177" s="3"/>
       <c r="F177" s="2"/>
       <c r="G177" s="3"/>
       <c r="H177" s="2"/>
-    </row>
-    <row r="178" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D178" s="2"/>
+      <c r="I177" s="6"/>
+    </row>
+    <row r="178" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D178" s="2">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
       <c r="E178" s="3"/>
       <c r="F178" s="2"/>
       <c r="G178" s="3"/>
       <c r="H178" s="2"/>
-    </row>
-    <row r="179" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D179" s="2"/>
+      <c r="I178" s="6"/>
+    </row>
+    <row r="179" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D179" s="2">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
       <c r="E179" s="3"/>
       <c r="F179" s="2"/>
       <c r="G179" s="3"/>
       <c r="H179" s="2"/>
-    </row>
-    <row r="180" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D180" s="2"/>
+      <c r="I179" s="6"/>
+    </row>
+    <row r="180" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D180" s="2">
+        <f t="shared" si="2"/>
+        <v>177</v>
+      </c>
       <c r="E180" s="3"/>
       <c r="F180" s="2"/>
       <c r="G180" s="3"/>
       <c r="H180" s="2"/>
-    </row>
-    <row r="181" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D181" s="2"/>
+      <c r="I180" s="6"/>
+    </row>
+    <row r="181" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D181" s="2">
+        <f t="shared" si="2"/>
+        <v>178</v>
+      </c>
       <c r="E181" s="3"/>
       <c r="F181" s="2"/>
       <c r="G181" s="3"/>
       <c r="H181" s="2"/>
-    </row>
-    <row r="182" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D182" s="2"/>
+      <c r="I181" s="6"/>
+    </row>
+    <row r="182" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D182" s="2">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
       <c r="E182" s="3"/>
       <c r="F182" s="2"/>
       <c r="G182" s="3"/>
       <c r="H182" s="2"/>
-    </row>
-    <row r="183" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D183" s="2"/>
+      <c r="I182" s="6"/>
+    </row>
+    <row r="183" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D183" s="2">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
       <c r="E183" s="3"/>
       <c r="F183" s="2"/>
       <c r="G183" s="3"/>
       <c r="H183" s="2"/>
-    </row>
-    <row r="184" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D184" s="2"/>
+      <c r="I183" s="6"/>
+    </row>
+    <row r="184" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D184" s="2">
+        <f t="shared" si="2"/>
+        <v>181</v>
+      </c>
       <c r="E184" s="3"/>
       <c r="F184" s="2"/>
       <c r="G184" s="3"/>
       <c r="H184" s="2"/>
-    </row>
-    <row r="185" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D185" s="2"/>
+      <c r="I184" s="6"/>
+    </row>
+    <row r="185" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D185" s="2">
+        <f t="shared" si="2"/>
+        <v>182</v>
+      </c>
       <c r="E185" s="3"/>
       <c r="F185" s="2"/>
       <c r="G185" s="3"/>
       <c r="H185" s="2"/>
-    </row>
-    <row r="186" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D186" s="2"/>
+      <c r="I185" s="6"/>
+    </row>
+    <row r="186" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D186" s="2">
+        <f t="shared" si="2"/>
+        <v>183</v>
+      </c>
       <c r="E186" s="3"/>
       <c r="F186" s="2"/>
       <c r="G186" s="3"/>
       <c r="H186" s="2"/>
-    </row>
-    <row r="187" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D187" s="2"/>
+      <c r="I186" s="6"/>
+    </row>
+    <row r="187" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D187" s="2">
+        <f t="shared" si="2"/>
+        <v>184</v>
+      </c>
       <c r="E187" s="3"/>
       <c r="F187" s="2"/>
       <c r="G187" s="3"/>
       <c r="H187" s="2"/>
-    </row>
-    <row r="188" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D188" s="2"/>
+      <c r="I187" s="6"/>
+    </row>
+    <row r="188" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D188" s="2">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
       <c r="E188" s="3"/>
       <c r="F188" s="2"/>
       <c r="G188" s="3"/>
       <c r="H188" s="2"/>
-    </row>
-    <row r="189" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D189" s="2"/>
+      <c r="I188" s="6"/>
+    </row>
+    <row r="189" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D189" s="2">
+        <f t="shared" si="2"/>
+        <v>186</v>
+      </c>
       <c r="E189" s="3"/>
       <c r="F189" s="2"/>
       <c r="G189" s="3"/>
       <c r="H189" s="2"/>
-    </row>
-    <row r="190" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D190" s="2"/>
+      <c r="I189" s="6"/>
+    </row>
+    <row r="190" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D190" s="2">
+        <f t="shared" si="2"/>
+        <v>187</v>
+      </c>
       <c r="E190" s="3"/>
       <c r="F190" s="2"/>
       <c r="G190" s="3"/>
       <c r="H190" s="2"/>
-    </row>
-    <row r="191" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D191" s="2"/>
+      <c r="I190" s="6"/>
+    </row>
+    <row r="191" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D191" s="2">
+        <f t="shared" si="2"/>
+        <v>188</v>
+      </c>
       <c r="E191" s="3"/>
       <c r="F191" s="2"/>
       <c r="G191" s="3"/>
       <c r="H191" s="2"/>
-    </row>
-    <row r="192" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D192" s="2"/>
+      <c r="I191" s="6"/>
+    </row>
+    <row r="192" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D192" s="2">
+        <f t="shared" si="2"/>
+        <v>189</v>
+      </c>
       <c r="E192" s="3"/>
       <c r="F192" s="2"/>
       <c r="G192" s="3"/>
       <c r="H192" s="2"/>
-    </row>
-    <row r="193" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D193" s="2"/>
+      <c r="I192" s="6"/>
+    </row>
+    <row r="193" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D193" s="2">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
       <c r="E193" s="3"/>
       <c r="F193" s="2"/>
       <c r="G193" s="3"/>
       <c r="H193" s="2"/>
-    </row>
-    <row r="194" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D194" s="2"/>
+      <c r="I193" s="6"/>
+    </row>
+    <row r="194" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D194" s="2">
+        <f t="shared" si="2"/>
+        <v>191</v>
+      </c>
       <c r="E194" s="3"/>
       <c r="F194" s="2"/>
       <c r="G194" s="3"/>
       <c r="H194" s="2"/>
-    </row>
-    <row r="195" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D195" s="2"/>
+      <c r="I194" s="6"/>
+    </row>
+    <row r="195" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D195" s="2">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
       <c r="E195" s="3"/>
       <c r="F195" s="2"/>
       <c r="G195" s="3"/>
       <c r="H195" s="2"/>
-    </row>
-    <row r="196" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D196" s="2"/>
+      <c r="I195" s="6"/>
+    </row>
+    <row r="196" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D196" s="2">
+        <f t="shared" si="2"/>
+        <v>193</v>
+      </c>
       <c r="E196" s="3"/>
       <c r="F196" s="2"/>
       <c r="G196" s="3"/>
       <c r="H196" s="2"/>
-    </row>
-    <row r="197" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D197" s="2"/>
+      <c r="I196" s="6"/>
+    </row>
+    <row r="197" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D197" s="2">
+        <f t="shared" si="2"/>
+        <v>194</v>
+      </c>
       <c r="E197" s="3"/>
       <c r="F197" s="2"/>
       <c r="G197" s="3"/>
       <c r="H197" s="2"/>
-    </row>
-    <row r="198" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D198" s="2"/>
+      <c r="I197" s="6"/>
+    </row>
+    <row r="198" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D198" s="2">
+        <f t="shared" si="2"/>
+        <v>195</v>
+      </c>
       <c r="E198" s="3"/>
       <c r="F198" s="2"/>
       <c r="G198" s="3"/>
       <c r="H198" s="2"/>
-    </row>
-    <row r="199" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D199" s="2"/>
+      <c r="I198" s="6"/>
+    </row>
+    <row r="199" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D199" s="2">
+        <f t="shared" ref="D199:D200" si="3">D198+1</f>
+        <v>196</v>
+      </c>
       <c r="E199" s="3"/>
       <c r="F199" s="2"/>
       <c r="G199" s="3"/>
       <c r="H199" s="2"/>
-    </row>
-    <row r="200" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D200" s="2"/>
-      <c r="E200" s="3"/>
-      <c r="F200" s="2"/>
-      <c r="G200" s="3"/>
-      <c r="H200" s="2"/>
+      <c r="I199" s="6"/>
+    </row>
+    <row r="200" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D200" s="8">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="E200" s="9"/>
+      <c r="F200" s="8"/>
+      <c r="G200" s="9"/>
+      <c r="H200" s="8"/>
+      <c r="I200" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agregaron referencias para las pruebas Se agrego ejemplo de plantilla de usabilidad
</commit_message>
<xml_diff>
--- a/extras/docs/Plantilla para Revision de Software.xlsx
+++ b/extras/docs/Plantilla para Revision de Software.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28515" windowHeight="12855"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Usabilidad" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Error</t>
   </si>
@@ -56,12 +56,111 @@
   <si>
     <t>Fecha de revision</t>
   </si>
+  <si>
+    <t>Identidad Corporativa</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>¿La portada del Sitio refleja la identidad y pertenencia de la institución?</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>¿Existen elementos de la imagen corporativa del Gobierno en la Portada de su Sitio? ¿Se repiten en todas las páginas?</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>¿El logotipo del Gobierno ha sido incluido en un lugar importante en la Portada y en las páginas interiores del Sitio?</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>¿Todas las páginas cuentan con un título que indique el nombre de la institución e información de contactos virtuales y físicos al pie de la página?</t>
+  </si>
+  <si>
+    <t>Utilidad del Sitio Web</t>
+  </si>
+  <si>
+    <t>1.¿El Sitio ofrece información sobre las actividades y servicios más recientes e importantes que está llevando a cabo la institución?</t>
+  </si>
+  <si>
+    <t>2.¿Los usuarios pueden encontrar fácilmente en la portada la información acerca de las actividades y servicios más importantes de la institución?</t>
+  </si>
+  <si>
+    <t>Navegación</t>
+  </si>
+  <si>
+    <t>1.¿El diseño del Sitio es eficiente, rápido e intuitivo?</t>
+  </si>
+  <si>
+    <t>2.¿Aparece el menú de navegación en un lugar destacado? ¿Se ve fácilmente?3.¿Verificó la consistencia de todos los enlaces?4.¿El Sitio cuenta con un mapa o buscador que facilite el acceso directo a los contenidos?5.¿El Sitio mantiene una navegación consistente y coherente en todas las pantallas?</t>
+  </si>
+  <si>
+    <t>Visibilidad del estado del sistema</t>
+  </si>
+  <si>
+    <t>1.¿Se informa al usuario claramente el área del Sitio que está visitando?</t>
+  </si>
+  <si>
+    <t>2.¿El Sitio Web diferencia entre enlaces visitados y enlaces por visitar?3.En caso de servicios o trámites en línea, ¿ofrece información de cuántos pasos faltan para terminar?</t>
+  </si>
+  <si>
+    <t>Consistencia y cumplimiento de estándares</t>
+  </si>
+  <si>
+    <t>1.¿El HTML del Sitio ha sido validado satisfactoriamente según w3c.org?</t>
+  </si>
+  <si>
+    <t>2.¿El o los archivos de Hojas de estilo (CSS) han sido aprobados según w3c.org?3.¿Comprobó la consistencia de Links usando el verificador de w3c.org?</t>
+  </si>
+  <si>
+    <t>Atención de errores</t>
+  </si>
+  <si>
+    <t>1.¿Usa Javascript para validar formularios durante su llenado y antes de enviarlos?</t>
+  </si>
+  <si>
+    <t>2.¿Usa elementos destacados para indicar los campos obligatorios dentro de un formulario?3.¿Después de que ocurre un error, es fácil volver a la página donde se encontraba antes que se produjese o entrega recomendaciones de los pasos a seguir?</t>
+  </si>
+  <si>
+    <t>Estética y diseño</t>
+  </si>
+  <si>
+    <t>1.¿Usa jerarquías visuales para determinar lo importante con una sola mirada?</t>
+  </si>
+  <si>
+    <t>2.¿Las imágenes tienen tamaños adecuados que no dificultan el acceso a las páginas?3.¿Las imágenes tienen etiqueta ALT en el código HTML para facilitar la navegación?</t>
+  </si>
+  <si>
+    <t>Ayuda ante errores</t>
+  </si>
+  <si>
+    <t>1.En caso de errores de consistencia dentro del sitio, ¿se ofrece un mensaje de personalizado mediante una página explicativa?, (Por ejemplo: Error 404 para página inexistente)</t>
+  </si>
+  <si>
+    <t>2.¿Entrega información de contacto fuera de Internet? (Por ejemplo: teléfono institucional, fono 600, mesa de ayuda, OIRS)3.¿Ofrece área de Preguntas Frecuentes con datos de ayuda a usuarios?2.¿Ofrece páginas de ayuda que explican cómo usar el Sitio?</t>
+  </si>
+  <si>
+    <t>Retroalimentación (Feedback)</t>
+  </si>
+  <si>
+    <t>1.¿Puede el usuario ponerse en contacto con el encargado del Sitio Web para hacer sugerencias o comentarios?</t>
+  </si>
+  <si>
+    <t>2.¿Funcionan correctamente los formularios de contacto?, ¿Ha probado cada uno de ellos?3.¿Hay alguien encargado de recibir y contestar estos mensajes?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +182,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14.3"/>
+      <color rgb="FF00A9C2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -184,6 +294,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -196,6 +315,2531 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="1181100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="1181100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="1943100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="AutoShape 4" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="1943100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1029" name="AutoShape 5" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="2705100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="AutoShape 6" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="2705100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1031" name="AutoShape 7" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="3467100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="AutoShape 8" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="3467100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1033" name="AutoShape 9" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="4267200"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1034" name="AutoShape 10" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="4267200"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1035" name="AutoShape 11" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="4267200"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1036" name="AutoShape 12" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1247775" y="4267200"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1037" name="AutoShape 13" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1038" name="AutoShape 14" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1039" name="AutoShape 15" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1040" name="AutoShape 16" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1247775" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1041" name="AutoShape 17" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1042" name="AutoShape 18" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1571625" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1043" name="AutoShape 19" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1733550" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1044" name="AutoShape 20" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1895475" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1045" name="AutoShape 21" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2057400" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1046" name="AutoShape 22" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2219325" y="5067300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1047" name="AutoShape 23" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="5867400"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1048" name="AutoShape 24" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="5867400"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1049" name="AutoShape 25" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="5867400"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1050" name="AutoShape 26" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1247775" y="5867400"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1051" name="AutoShape 27" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="5867400"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1052" name="AutoShape 28" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1571625" y="5867400"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1053" name="AutoShape 29" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="6667500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1054" name="AutoShape 30" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="6667500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1055" name="AutoShape 31" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="6667500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1056" name="AutoShape 32" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1247775" y="6667500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1057" name="AutoShape 33" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="6667500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1058" name="AutoShape 34" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1571625" y="6667500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1059" name="AutoShape 35" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="7467600"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1060" name="AutoShape 36" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="7467600"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1061" name="AutoShape 37" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="7467600"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1062" name="AutoShape 38" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1247775" y="7467600"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1063" name="AutoShape 39" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="7467600"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1064" name="AutoShape 40" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1571625" y="7467600"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1065" name="AutoShape 41" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="8267700"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1066" name="AutoShape 42" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="8267700"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1067" name="AutoShape 43" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="8267700"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1068" name="AutoShape 44" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1247775" y="8267700"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1069" name="AutoShape 45" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="8267700"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1070" name="AutoShape 46" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1571625" y="8267700"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1071" name="AutoShape 47" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="9067800"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1072" name="AutoShape 48" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="9067800"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1073" name="AutoShape 49" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="9067800"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1074" name="AutoShape 50" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1247775" y="9067800"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1075" name="AutoShape 51" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="9067800"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1076" name="AutoShape 52" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1571625" y="9067800"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1077" name="AutoShape 53" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1733550" y="9067800"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1078" name="AutoShape 54" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1895475" y="9067800"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1079" name="AutoShape 55" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="9867900"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1080" name="AutoShape 56" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="9867900"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1081" name="AutoShape 57" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="9867900"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1082" name="AutoShape 58" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1247775" y="9867900"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1083" name="AutoShape 59" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="9867900"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1084" name="AutoShape 60" descr="Sí"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1571625" y="9867900"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,18 +3131,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="38" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:9" ht="39" customHeight="1">
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
@@ -518,7 +3162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:9">
       <c r="D4" s="2">
         <v>1</v>
       </c>
@@ -528,7 +3172,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:9">
       <c r="D5" s="2">
         <f>D4+1</f>
         <v>2</v>
@@ -539,7 +3183,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:9">
       <c r="D6" s="2">
         <f t="shared" ref="D6:D69" si="0">D5+1</f>
         <v>3</v>
@@ -550,7 +3194,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:9">
       <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -561,7 +3205,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:9">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -572,7 +3216,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:9">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -583,7 +3227,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:9">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -594,7 +3238,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:9">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -605,7 +3249,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:9">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -616,7 +3260,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:9">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -627,7 +3271,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:9">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -638,7 +3282,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:9">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -649,7 +3293,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:9">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -660,7 +3304,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:9">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -671,7 +3315,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:9">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -682,7 +3326,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:9">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -693,7 +3337,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:9">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -704,7 +3348,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:9">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -715,7 +3359,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:9">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -726,7 +3370,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:9">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -737,7 +3381,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:9">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -748,7 +3392,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:9">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -759,7 +3403,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:9">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -770,7 +3414,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:9">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -781,7 +3425,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:9">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -792,7 +3436,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:9">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -803,7 +3447,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:9">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -814,7 +3458,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:9">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -825,7 +3469,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:9">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -836,7 +3480,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:9">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -847,7 +3491,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:9">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -858,7 +3502,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:9">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -869,7 +3513,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:9">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -880,7 +3524,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:9">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -891,7 +3535,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:9">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -902,7 +3546,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:9">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -913,7 +3557,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:9">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -924,7 +3568,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:9">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -935,7 +3579,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:9">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -946,7 +3590,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:9">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -957,7 +3601,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:9">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -968,7 +3612,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:9">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -979,7 +3623,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:9">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -990,7 +3634,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:9">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1001,7 +3645,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:9">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1012,7 +3656,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:9">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1023,7 +3667,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:9">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1034,7 +3678,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:9">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1045,7 +3689,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:9">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1056,7 +3700,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:9">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1067,7 +3711,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:9">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1078,7 +3722,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:9">
       <c r="D55" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1089,7 +3733,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:9">
       <c r="D56" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1100,7 +3744,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:9">
       <c r="D57" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1111,7 +3755,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:9">
       <c r="D58" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1122,7 +3766,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:9">
       <c r="D59" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1133,7 +3777,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:9">
       <c r="D60" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1144,7 +3788,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:9">
       <c r="D61" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1155,7 +3799,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:9">
       <c r="D62" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1166,7 +3810,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:9">
       <c r="D63" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1177,7 +3821,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:9">
       <c r="D64" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1188,7 +3832,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:9">
       <c r="D65" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1199,7 +3843,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:9">
       <c r="D66" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1210,7 +3854,7 @@
       <c r="H66" s="2"/>
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:9">
       <c r="D67" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1221,7 +3865,7 @@
       <c r="H67" s="2"/>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:9">
       <c r="D68" s="2">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1232,7 +3876,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:9">
       <c r="D69" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -1243,7 +3887,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:9">
       <c r="D70" s="2">
         <f>D69+1</f>
         <v>67</v>
@@ -1254,7 +3898,7 @@
       <c r="H70" s="2"/>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:9">
       <c r="D71" s="2">
         <f t="shared" ref="D71:D134" si="1">D70+1</f>
         <v>68</v>
@@ -1265,7 +3909,7 @@
       <c r="H71" s="2"/>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:9">
       <c r="D72" s="2">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -1276,7 +3920,7 @@
       <c r="H72" s="2"/>
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:9">
       <c r="D73" s="2">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -1287,7 +3931,7 @@
       <c r="H73" s="2"/>
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:9">
       <c r="D74" s="2">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -1298,7 +3942,7 @@
       <c r="H74" s="2"/>
       <c r="I74" s="6"/>
     </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:9">
       <c r="D75" s="2">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -1309,7 +3953,7 @@
       <c r="H75" s="2"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:9">
       <c r="D76" s="2">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -1320,7 +3964,7 @@
       <c r="H76" s="2"/>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:9">
       <c r="D77" s="2">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -1331,7 +3975,7 @@
       <c r="H77" s="2"/>
       <c r="I77" s="6"/>
     </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:9">
       <c r="D78" s="2">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -1342,7 +3986,7 @@
       <c r="H78" s="2"/>
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:9">
       <c r="D79" s="2">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -1353,7 +3997,7 @@
       <c r="H79" s="2"/>
       <c r="I79" s="6"/>
     </row>
-    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:9">
       <c r="D80" s="2">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -1364,7 +4008,7 @@
       <c r="H80" s="2"/>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:9">
       <c r="D81" s="2">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -1375,7 +4019,7 @@
       <c r="H81" s="2"/>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:9">
       <c r="D82" s="2">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -1386,7 +4030,7 @@
       <c r="H82" s="2"/>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:9">
       <c r="D83" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -1397,7 +4041,7 @@
       <c r="H83" s="2"/>
       <c r="I83" s="6"/>
     </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:9">
       <c r="D84" s="2">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -1408,7 +4052,7 @@
       <c r="H84" s="2"/>
       <c r="I84" s="6"/>
     </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:9">
       <c r="D85" s="2">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -1419,7 +4063,7 @@
       <c r="H85" s="2"/>
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:9">
       <c r="D86" s="2">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -1430,7 +4074,7 @@
       <c r="H86" s="2"/>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:9">
       <c r="D87" s="2">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -1441,7 +4085,7 @@
       <c r="H87" s="2"/>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:9">
       <c r="D88" s="2">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -1452,7 +4096,7 @@
       <c r="H88" s="2"/>
       <c r="I88" s="6"/>
     </row>
-    <row r="89" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:9">
       <c r="D89" s="2">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -1463,7 +4107,7 @@
       <c r="H89" s="2"/>
       <c r="I89" s="6"/>
     </row>
-    <row r="90" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:9">
       <c r="D90" s="2">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -1474,7 +4118,7 @@
       <c r="H90" s="2"/>
       <c r="I90" s="6"/>
     </row>
-    <row r="91" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:9">
       <c r="D91" s="2">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -1485,7 +4129,7 @@
       <c r="H91" s="2"/>
       <c r="I91" s="6"/>
     </row>
-    <row r="92" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:9">
       <c r="D92" s="2">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -1496,7 +4140,7 @@
       <c r="H92" s="2"/>
       <c r="I92" s="6"/>
     </row>
-    <row r="93" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:9">
       <c r="D93" s="2">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -1507,7 +4151,7 @@
       <c r="H93" s="2"/>
       <c r="I93" s="6"/>
     </row>
-    <row r="94" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:9">
       <c r="D94" s="2">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -1518,7 +4162,7 @@
       <c r="H94" s="2"/>
       <c r="I94" s="6"/>
     </row>
-    <row r="95" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:9">
       <c r="D95" s="2">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -1529,7 +4173,7 @@
       <c r="H95" s="2"/>
       <c r="I95" s="6"/>
     </row>
-    <row r="96" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:9">
       <c r="D96" s="2">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -1540,7 +4184,7 @@
       <c r="H96" s="2"/>
       <c r="I96" s="6"/>
     </row>
-    <row r="97" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:9">
       <c r="D97" s="2">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -1551,7 +4195,7 @@
       <c r="H97" s="2"/>
       <c r="I97" s="6"/>
     </row>
-    <row r="98" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:9">
       <c r="D98" s="2">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -1562,7 +4206,7 @@
       <c r="H98" s="2"/>
       <c r="I98" s="6"/>
     </row>
-    <row r="99" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:9">
       <c r="D99" s="2">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -1573,7 +4217,7 @@
       <c r="H99" s="2"/>
       <c r="I99" s="6"/>
     </row>
-    <row r="100" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:9">
       <c r="D100" s="2">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -1584,7 +4228,7 @@
       <c r="H100" s="2"/>
       <c r="I100" s="6"/>
     </row>
-    <row r="101" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:9">
       <c r="D101" s="2">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -1595,7 +4239,7 @@
       <c r="H101" s="2"/>
       <c r="I101" s="6"/>
     </row>
-    <row r="102" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:9">
       <c r="D102" s="2">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -1606,7 +4250,7 @@
       <c r="H102" s="2"/>
       <c r="I102" s="6"/>
     </row>
-    <row r="103" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:9">
       <c r="D103" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -1617,7 +4261,7 @@
       <c r="H103" s="2"/>
       <c r="I103" s="6"/>
     </row>
-    <row r="104" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:9">
       <c r="D104" s="2">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -1628,7 +4272,7 @@
       <c r="H104" s="2"/>
       <c r="I104" s="6"/>
     </row>
-    <row r="105" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:9">
       <c r="D105" s="2">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -1639,7 +4283,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="6"/>
     </row>
-    <row r="106" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:9">
       <c r="D106" s="2">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -1650,7 +4294,7 @@
       <c r="H106" s="2"/>
       <c r="I106" s="6"/>
     </row>
-    <row r="107" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:9">
       <c r="D107" s="2">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -1661,7 +4305,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="6"/>
     </row>
-    <row r="108" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:9">
       <c r="D108" s="2">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -1672,7 +4316,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="6"/>
     </row>
-    <row r="109" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:9">
       <c r="D109" s="2">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -1683,7 +4327,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="6"/>
     </row>
-    <row r="110" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:9">
       <c r="D110" s="2">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -1694,7 +4338,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="6"/>
     </row>
-    <row r="111" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:9">
       <c r="D111" s="2">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -1705,7 +4349,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="6"/>
     </row>
-    <row r="112" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:9">
       <c r="D112" s="2">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -1716,7 +4360,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="6"/>
     </row>
-    <row r="113" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:9">
       <c r="D113" s="2">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -1727,7 +4371,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="6"/>
     </row>
-    <row r="114" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:9">
       <c r="D114" s="2">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -1738,7 +4382,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="6"/>
     </row>
-    <row r="115" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:9">
       <c r="D115" s="2">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -1749,7 +4393,7 @@
       <c r="H115" s="2"/>
       <c r="I115" s="6"/>
     </row>
-    <row r="116" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:9">
       <c r="D116" s="2">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -1760,7 +4404,7 @@
       <c r="H116" s="2"/>
       <c r="I116" s="6"/>
     </row>
-    <row r="117" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:9">
       <c r="D117" s="2">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -1771,7 +4415,7 @@
       <c r="H117" s="2"/>
       <c r="I117" s="6"/>
     </row>
-    <row r="118" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:9">
       <c r="D118" s="2">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -1782,7 +4426,7 @@
       <c r="H118" s="2"/>
       <c r="I118" s="6"/>
     </row>
-    <row r="119" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:9">
       <c r="D119" s="2">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -1793,7 +4437,7 @@
       <c r="H119" s="2"/>
       <c r="I119" s="6"/>
     </row>
-    <row r="120" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:9">
       <c r="D120" s="2">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1804,7 +4448,7 @@
       <c r="H120" s="2"/>
       <c r="I120" s="6"/>
     </row>
-    <row r="121" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:9">
       <c r="D121" s="2">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -1815,7 +4459,7 @@
       <c r="H121" s="2"/>
       <c r="I121" s="6"/>
     </row>
-    <row r="122" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:9">
       <c r="D122" s="2">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -1826,7 +4470,7 @@
       <c r="H122" s="2"/>
       <c r="I122" s="6"/>
     </row>
-    <row r="123" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:9">
       <c r="D123" s="2">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -1837,7 +4481,7 @@
       <c r="H123" s="2"/>
       <c r="I123" s="6"/>
     </row>
-    <row r="124" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:9">
       <c r="D124" s="2">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -1848,7 +4492,7 @@
       <c r="H124" s="2"/>
       <c r="I124" s="6"/>
     </row>
-    <row r="125" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:9">
       <c r="D125" s="2">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -1859,7 +4503,7 @@
       <c r="H125" s="2"/>
       <c r="I125" s="6"/>
     </row>
-    <row r="126" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:9">
       <c r="D126" s="2">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -1870,7 +4514,7 @@
       <c r="H126" s="2"/>
       <c r="I126" s="6"/>
     </row>
-    <row r="127" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:9">
       <c r="D127" s="2">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -1881,7 +4525,7 @@
       <c r="H127" s="2"/>
       <c r="I127" s="6"/>
     </row>
-    <row r="128" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:9">
       <c r="D128" s="2">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -1892,7 +4536,7 @@
       <c r="H128" s="2"/>
       <c r="I128" s="6"/>
     </row>
-    <row r="129" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:9">
       <c r="D129" s="2">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -1903,7 +4547,7 @@
       <c r="H129" s="2"/>
       <c r="I129" s="6"/>
     </row>
-    <row r="130" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:9">
       <c r="D130" s="2">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -1914,7 +4558,7 @@
       <c r="H130" s="2"/>
       <c r="I130" s="6"/>
     </row>
-    <row r="131" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:9">
       <c r="D131" s="2">
         <f t="shared" si="1"/>
         <v>128</v>
@@ -1925,7 +4569,7 @@
       <c r="H131" s="2"/>
       <c r="I131" s="6"/>
     </row>
-    <row r="132" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:9">
       <c r="D132" s="2">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -1936,7 +4580,7 @@
       <c r="H132" s="2"/>
       <c r="I132" s="6"/>
     </row>
-    <row r="133" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:9">
       <c r="D133" s="2">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -1947,7 +4591,7 @@
       <c r="H133" s="2"/>
       <c r="I133" s="6"/>
     </row>
-    <row r="134" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:9">
       <c r="D134" s="2">
         <f t="shared" si="1"/>
         <v>131</v>
@@ -1958,7 +4602,7 @@
       <c r="H134" s="2"/>
       <c r="I134" s="6"/>
     </row>
-    <row r="135" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:9">
       <c r="D135" s="2">
         <f t="shared" ref="D135:D198" si="2">D134+1</f>
         <v>132</v>
@@ -1969,7 +4613,7 @@
       <c r="H135" s="2"/>
       <c r="I135" s="6"/>
     </row>
-    <row r="136" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:9">
       <c r="D136" s="2">
         <f t="shared" si="2"/>
         <v>133</v>
@@ -1980,7 +4624,7 @@
       <c r="H136" s="2"/>
       <c r="I136" s="6"/>
     </row>
-    <row r="137" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:9">
       <c r="D137" s="2">
         <f t="shared" si="2"/>
         <v>134</v>
@@ -1991,7 +4635,7 @@
       <c r="H137" s="2"/>
       <c r="I137" s="6"/>
     </row>
-    <row r="138" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:9">
       <c r="D138" s="2">
         <f t="shared" si="2"/>
         <v>135</v>
@@ -2002,7 +4646,7 @@
       <c r="H138" s="2"/>
       <c r="I138" s="6"/>
     </row>
-    <row r="139" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:9">
       <c r="D139" s="2">
         <f t="shared" si="2"/>
         <v>136</v>
@@ -2013,7 +4657,7 @@
       <c r="H139" s="2"/>
       <c r="I139" s="6"/>
     </row>
-    <row r="140" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:9">
       <c r="D140" s="2">
         <f t="shared" si="2"/>
         <v>137</v>
@@ -2024,7 +4668,7 @@
       <c r="H140" s="2"/>
       <c r="I140" s="6"/>
     </row>
-    <row r="141" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:9">
       <c r="D141" s="2">
         <f t="shared" si="2"/>
         <v>138</v>
@@ -2035,7 +4679,7 @@
       <c r="H141" s="2"/>
       <c r="I141" s="6"/>
     </row>
-    <row r="142" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:9">
       <c r="D142" s="2">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -2046,7 +4690,7 @@
       <c r="H142" s="2"/>
       <c r="I142" s="6"/>
     </row>
-    <row r="143" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:9">
       <c r="D143" s="2">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -2057,7 +4701,7 @@
       <c r="H143" s="2"/>
       <c r="I143" s="6"/>
     </row>
-    <row r="144" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:9">
       <c r="D144" s="2">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -2068,7 +4712,7 @@
       <c r="H144" s="2"/>
       <c r="I144" s="6"/>
     </row>
-    <row r="145" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:9">
       <c r="D145" s="2">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -2079,7 +4723,7 @@
       <c r="H145" s="2"/>
       <c r="I145" s="6"/>
     </row>
-    <row r="146" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:9">
       <c r="D146" s="2">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -2090,7 +4734,7 @@
       <c r="H146" s="2"/>
       <c r="I146" s="6"/>
     </row>
-    <row r="147" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:9">
       <c r="D147" s="2">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -2101,7 +4745,7 @@
       <c r="H147" s="2"/>
       <c r="I147" s="6"/>
     </row>
-    <row r="148" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:9">
       <c r="D148" s="2">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -2112,7 +4756,7 @@
       <c r="H148" s="2"/>
       <c r="I148" s="6"/>
     </row>
-    <row r="149" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="4:9">
       <c r="D149" s="2">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -2123,7 +4767,7 @@
       <c r="H149" s="2"/>
       <c r="I149" s="6"/>
     </row>
-    <row r="150" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:9">
       <c r="D150" s="2">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -2134,7 +4778,7 @@
       <c r="H150" s="2"/>
       <c r="I150" s="6"/>
     </row>
-    <row r="151" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:9">
       <c r="D151" s="2">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -2145,7 +4789,7 @@
       <c r="H151" s="2"/>
       <c r="I151" s="6"/>
     </row>
-    <row r="152" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:9">
       <c r="D152" s="2">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -2156,7 +4800,7 @@
       <c r="H152" s="2"/>
       <c r="I152" s="6"/>
     </row>
-    <row r="153" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="4:9">
       <c r="D153" s="2">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -2167,7 +4811,7 @@
       <c r="H153" s="2"/>
       <c r="I153" s="6"/>
     </row>
-    <row r="154" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:9">
       <c r="D154" s="2">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -2178,7 +4822,7 @@
       <c r="H154" s="2"/>
       <c r="I154" s="6"/>
     </row>
-    <row r="155" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="4:9">
       <c r="D155" s="2">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -2189,7 +4833,7 @@
       <c r="H155" s="2"/>
       <c r="I155" s="6"/>
     </row>
-    <row r="156" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="4:9">
       <c r="D156" s="2">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -2200,7 +4844,7 @@
       <c r="H156" s="2"/>
       <c r="I156" s="6"/>
     </row>
-    <row r="157" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="4:9">
       <c r="D157" s="2">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -2211,7 +4855,7 @@
       <c r="H157" s="2"/>
       <c r="I157" s="6"/>
     </row>
-    <row r="158" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="4:9">
       <c r="D158" s="2">
         <f t="shared" si="2"/>
         <v>155</v>
@@ -2222,7 +4866,7 @@
       <c r="H158" s="2"/>
       <c r="I158" s="6"/>
     </row>
-    <row r="159" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:9">
       <c r="D159" s="2">
         <f t="shared" si="2"/>
         <v>156</v>
@@ -2233,7 +4877,7 @@
       <c r="H159" s="2"/>
       <c r="I159" s="6"/>
     </row>
-    <row r="160" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="4:9">
       <c r="D160" s="2">
         <f t="shared" si="2"/>
         <v>157</v>
@@ -2244,7 +4888,7 @@
       <c r="H160" s="2"/>
       <c r="I160" s="6"/>
     </row>
-    <row r="161" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="4:9">
       <c r="D161" s="2">
         <f t="shared" si="2"/>
         <v>158</v>
@@ -2255,7 +4899,7 @@
       <c r="H161" s="2"/>
       <c r="I161" s="6"/>
     </row>
-    <row r="162" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="4:9">
       <c r="D162" s="2">
         <f t="shared" si="2"/>
         <v>159</v>
@@ -2266,7 +4910,7 @@
       <c r="H162" s="2"/>
       <c r="I162" s="6"/>
     </row>
-    <row r="163" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="4:9">
       <c r="D163" s="2">
         <f t="shared" si="2"/>
         <v>160</v>
@@ -2277,7 +4921,7 @@
       <c r="H163" s="2"/>
       <c r="I163" s="6"/>
     </row>
-    <row r="164" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="4:9">
       <c r="D164" s="2">
         <f t="shared" si="2"/>
         <v>161</v>
@@ -2288,7 +4932,7 @@
       <c r="H164" s="2"/>
       <c r="I164" s="6"/>
     </row>
-    <row r="165" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="4:9">
       <c r="D165" s="2">
         <f t="shared" si="2"/>
         <v>162</v>
@@ -2299,7 +4943,7 @@
       <c r="H165" s="2"/>
       <c r="I165" s="6"/>
     </row>
-    <row r="166" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="4:9">
       <c r="D166" s="2">
         <f t="shared" si="2"/>
         <v>163</v>
@@ -2310,7 +4954,7 @@
       <c r="H166" s="2"/>
       <c r="I166" s="6"/>
     </row>
-    <row r="167" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="4:9">
       <c r="D167" s="2">
         <f t="shared" si="2"/>
         <v>164</v>
@@ -2321,7 +4965,7 @@
       <c r="H167" s="2"/>
       <c r="I167" s="6"/>
     </row>
-    <row r="168" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="4:9">
       <c r="D168" s="2">
         <f t="shared" si="2"/>
         <v>165</v>
@@ -2332,7 +4976,7 @@
       <c r="H168" s="2"/>
       <c r="I168" s="6"/>
     </row>
-    <row r="169" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="4:9">
       <c r="D169" s="2">
         <f t="shared" si="2"/>
         <v>166</v>
@@ -2343,7 +4987,7 @@
       <c r="H169" s="2"/>
       <c r="I169" s="6"/>
     </row>
-    <row r="170" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="4:9">
       <c r="D170" s="2">
         <f t="shared" si="2"/>
         <v>167</v>
@@ -2354,7 +4998,7 @@
       <c r="H170" s="2"/>
       <c r="I170" s="6"/>
     </row>
-    <row r="171" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="4:9">
       <c r="D171" s="2">
         <f t="shared" si="2"/>
         <v>168</v>
@@ -2365,7 +5009,7 @@
       <c r="H171" s="2"/>
       <c r="I171" s="6"/>
     </row>
-    <row r="172" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="4:9">
       <c r="D172" s="2">
         <f t="shared" si="2"/>
         <v>169</v>
@@ -2376,7 +5020,7 @@
       <c r="H172" s="2"/>
       <c r="I172" s="6"/>
     </row>
-    <row r="173" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="4:9">
       <c r="D173" s="2">
         <f t="shared" si="2"/>
         <v>170</v>
@@ -2387,7 +5031,7 @@
       <c r="H173" s="2"/>
       <c r="I173" s="6"/>
     </row>
-    <row r="174" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="4:9">
       <c r="D174" s="2">
         <f t="shared" si="2"/>
         <v>171</v>
@@ -2398,7 +5042,7 @@
       <c r="H174" s="2"/>
       <c r="I174" s="6"/>
     </row>
-    <row r="175" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="4:9">
       <c r="D175" s="2">
         <f t="shared" si="2"/>
         <v>172</v>
@@ -2409,7 +5053,7 @@
       <c r="H175" s="2"/>
       <c r="I175" s="6"/>
     </row>
-    <row r="176" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="4:9">
       <c r="D176" s="2">
         <f t="shared" si="2"/>
         <v>173</v>
@@ -2420,7 +5064,7 @@
       <c r="H176" s="2"/>
       <c r="I176" s="6"/>
     </row>
-    <row r="177" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="4:9">
       <c r="D177" s="2">
         <f t="shared" si="2"/>
         <v>174</v>
@@ -2431,7 +5075,7 @@
       <c r="H177" s="2"/>
       <c r="I177" s="6"/>
     </row>
-    <row r="178" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="4:9">
       <c r="D178" s="2">
         <f t="shared" si="2"/>
         <v>175</v>
@@ -2442,7 +5086,7 @@
       <c r="H178" s="2"/>
       <c r="I178" s="6"/>
     </row>
-    <row r="179" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="4:9">
       <c r="D179" s="2">
         <f t="shared" si="2"/>
         <v>176</v>
@@ -2453,7 +5097,7 @@
       <c r="H179" s="2"/>
       <c r="I179" s="6"/>
     </row>
-    <row r="180" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="4:9">
       <c r="D180" s="2">
         <f t="shared" si="2"/>
         <v>177</v>
@@ -2464,7 +5108,7 @@
       <c r="H180" s="2"/>
       <c r="I180" s="6"/>
     </row>
-    <row r="181" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="4:9">
       <c r="D181" s="2">
         <f t="shared" si="2"/>
         <v>178</v>
@@ -2475,7 +5119,7 @@
       <c r="H181" s="2"/>
       <c r="I181" s="6"/>
     </row>
-    <row r="182" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="4:9">
       <c r="D182" s="2">
         <f t="shared" si="2"/>
         <v>179</v>
@@ -2486,7 +5130,7 @@
       <c r="H182" s="2"/>
       <c r="I182" s="6"/>
     </row>
-    <row r="183" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="4:9">
       <c r="D183" s="2">
         <f t="shared" si="2"/>
         <v>180</v>
@@ -2497,7 +5141,7 @@
       <c r="H183" s="2"/>
       <c r="I183" s="6"/>
     </row>
-    <row r="184" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="4:9">
       <c r="D184" s="2">
         <f t="shared" si="2"/>
         <v>181</v>
@@ -2508,7 +5152,7 @@
       <c r="H184" s="2"/>
       <c r="I184" s="6"/>
     </row>
-    <row r="185" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="4:9">
       <c r="D185" s="2">
         <f t="shared" si="2"/>
         <v>182</v>
@@ -2519,7 +5163,7 @@
       <c r="H185" s="2"/>
       <c r="I185" s="6"/>
     </row>
-    <row r="186" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="4:9">
       <c r="D186" s="2">
         <f t="shared" si="2"/>
         <v>183</v>
@@ -2530,7 +5174,7 @@
       <c r="H186" s="2"/>
       <c r="I186" s="6"/>
     </row>
-    <row r="187" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="4:9">
       <c r="D187" s="2">
         <f t="shared" si="2"/>
         <v>184</v>
@@ -2541,7 +5185,7 @@
       <c r="H187" s="2"/>
       <c r="I187" s="6"/>
     </row>
-    <row r="188" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="4:9">
       <c r="D188" s="2">
         <f t="shared" si="2"/>
         <v>185</v>
@@ -2552,7 +5196,7 @@
       <c r="H188" s="2"/>
       <c r="I188" s="6"/>
     </row>
-    <row r="189" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="4:9">
       <c r="D189" s="2">
         <f t="shared" si="2"/>
         <v>186</v>
@@ -2563,7 +5207,7 @@
       <c r="H189" s="2"/>
       <c r="I189" s="6"/>
     </row>
-    <row r="190" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="4:9">
       <c r="D190" s="2">
         <f t="shared" si="2"/>
         <v>187</v>
@@ -2574,7 +5218,7 @@
       <c r="H190" s="2"/>
       <c r="I190" s="6"/>
     </row>
-    <row r="191" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="4:9">
       <c r="D191" s="2">
         <f t="shared" si="2"/>
         <v>188</v>
@@ -2585,7 +5229,7 @@
       <c r="H191" s="2"/>
       <c r="I191" s="6"/>
     </row>
-    <row r="192" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="4:9">
       <c r="D192" s="2">
         <f t="shared" si="2"/>
         <v>189</v>
@@ -2596,7 +5240,7 @@
       <c r="H192" s="2"/>
       <c r="I192" s="6"/>
     </row>
-    <row r="193" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="4:9">
       <c r="D193" s="2">
         <f t="shared" si="2"/>
         <v>190</v>
@@ -2607,7 +5251,7 @@
       <c r="H193" s="2"/>
       <c r="I193" s="6"/>
     </row>
-    <row r="194" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="4:9">
       <c r="D194" s="2">
         <f t="shared" si="2"/>
         <v>191</v>
@@ -2618,7 +5262,7 @@
       <c r="H194" s="2"/>
       <c r="I194" s="6"/>
     </row>
-    <row r="195" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="4:9">
       <c r="D195" s="2">
         <f t="shared" si="2"/>
         <v>192</v>
@@ -2629,7 +5273,7 @@
       <c r="H195" s="2"/>
       <c r="I195" s="6"/>
     </row>
-    <row r="196" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="4:9">
       <c r="D196" s="2">
         <f t="shared" si="2"/>
         <v>193</v>
@@ -2640,7 +5284,7 @@
       <c r="H196" s="2"/>
       <c r="I196" s="6"/>
     </row>
-    <row r="197" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="4:9">
       <c r="D197" s="2">
         <f t="shared" si="2"/>
         <v>194</v>
@@ -2651,7 +5295,7 @@
       <c r="H197" s="2"/>
       <c r="I197" s="6"/>
     </row>
-    <row r="198" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="4:9">
       <c r="D198" s="2">
         <f t="shared" si="2"/>
         <v>195</v>
@@ -2662,7 +5306,7 @@
       <c r="H198" s="2"/>
       <c r="I198" s="6"/>
     </row>
-    <row r="199" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="4:9">
       <c r="D199" s="2">
         <f t="shared" ref="D199:D200" si="3">D198+1</f>
         <v>196</v>
@@ -2673,7 +5317,7 @@
       <c r="H199" s="2"/>
       <c r="I199" s="6"/>
     </row>
-    <row r="200" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="4:9">
       <c r="D200" s="8">
         <f t="shared" si="3"/>
         <v>197</v>
@@ -2709,18 +5353,227 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" ht="18">
+      <c r="B3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="2:2" ht="18">
+      <c r="B21" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25" spans="2:2" ht="18">
+      <c r="B25" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="2:2" ht="18">
+      <c r="B29" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="2:2" ht="18">
+      <c r="B33" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="2:2" ht="18">
+      <c r="B37" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="10"/>
+    </row>
+    <row r="41" spans="2:2" ht="18">
+      <c r="B41" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="10"/>
+    </row>
+    <row r="45" spans="2:2" ht="18">
+      <c r="B45" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="10"/>
+    </row>
+    <row r="49" spans="2:2" ht="18">
+      <c r="B49" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -2728,7 +5581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -2736,7 +5589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2744,7 +5597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -2756,16 +5609,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego pendiente Se borraron archivos que no se usan
</commit_message>
<xml_diff>
--- a/extras/docs/Plantilla para Revision de Software.xlsx
+++ b/extras/docs/Plantilla para Revision de Software.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Error</t>
   </si>
@@ -58,21 +58,6 @@
   </si>
   <si>
     <t>Identidad Corporativa</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>¿La portada del Sitio refleja la identidad y pertenencia de la institución?</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>¿Existen elementos de la imagen corporativa del Gobierno en la Portada de su Sitio? ¿Se repiten en todas las páginas?</t>
-  </si>
-  <si>
-    <t>3.</t>
   </si>
   <si>
     <t>¿El logotipo del Gobierno ha sido incluido en un lugar importante en la Portada y en las páginas interiores del Sitio?</t>
@@ -154,6 +139,9 @@
   </si>
   <si>
     <t>2.¿Funcionan correctamente los formularios de contacto?, ¿Ha probado cada uno de ellos?3.¿Hay alguien encargado de recibir y contestar estos mensajes?</t>
+  </si>
+  <si>
+    <t>1. Se mantiene la identidad y pertenencia de la institucion?</t>
   </si>
 </sst>
 </file>
@@ -5355,8 +5343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5372,42 +5360,28 @@
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:2">
-      <c r="B8" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
+      <c r="B8" s="12"/>
     </row>
     <row r="12" spans="2:2">
-      <c r="B12" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="B12" s="12"/>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:2">
@@ -5415,17 +5389,17 @@
     </row>
     <row r="21" spans="2:2" ht="18">
       <c r="B21" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="2:2">
@@ -5433,17 +5407,17 @@
     </row>
     <row r="25" spans="2:2" ht="18">
       <c r="B25" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="2:2">
@@ -5451,17 +5425,17 @@
     </row>
     <row r="29" spans="2:2" ht="18">
       <c r="B29" s="11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:2">
@@ -5469,17 +5443,17 @@
     </row>
     <row r="33" spans="2:2" ht="18">
       <c r="B33" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="2:2">
@@ -5487,17 +5461,17 @@
     </row>
     <row r="37" spans="2:2" ht="18">
       <c r="B37" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="2:2">
@@ -5505,17 +5479,17 @@
     </row>
     <row r="41" spans="2:2" ht="18">
       <c r="B41" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="2:2">
@@ -5523,17 +5497,17 @@
     </row>
     <row r="45" spans="2:2" ht="18">
       <c r="B45" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="2:2">
@@ -5541,17 +5515,17 @@
     </row>
     <row r="49" spans="2:2" ht="18">
       <c r="B49" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>